<commit_message>
Updated sprint10 Stand-up Meeting templet.
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint10/Team05 Stand-up Meeting Sprint10.xlsx
+++ b/Project_Files/Sprint10/Team05 Stand-up Meeting Sprint10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/Sprint10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\Sprint10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_56FD0622E9534DA529C0F15AAB95F0106330DBA9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8710D898-0D98-4DE6-8B68-1BFEC49FDACD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6E5723-7079-4F33-BCD6-0F6F332CE815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -156,6 +156,27 @@
   </si>
   <si>
     <t>preparing slides for midterm presentation</t>
+  </si>
+  <si>
+    <t>2) I will prepare power point presentation slide on Intents for Workshop.</t>
+  </si>
+  <si>
+    <t>1) I have modified Event class and update Event class.</t>
+  </si>
+  <si>
+    <t>1) I have modified the model references and adapter references in Home Activity class</t>
+  </si>
+  <si>
+    <t>2) I will presenation on Intents during class time.</t>
+  </si>
+  <si>
+    <t>3) NA</t>
+  </si>
+  <si>
+    <t>1) I have wrote functionality using Intents.</t>
+  </si>
+  <si>
+    <t>2) I will prepare presentation slide for Midterm02.</t>
   </si>
 </sst>
 </file>
@@ -712,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1127,9 +1148,15 @@
       <c r="A14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1155,9 +1182,15 @@
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
       <c r="A15" s="10"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1183,9 +1216,15 @@
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>

</xml_diff>

<commit_message>
Update my process in these week
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint10/Team05 Stand-up Meeting Sprint10.xlsx
+++ b/Project_Files/Sprint10/Team05 Stand-up Meeting Sprint10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\Sprint10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\FreebiesforNewbies\Project_Files\Sprint10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7615154F-D884-43DD-AC13-AE784B8D3DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F4B581-3E84-41F3-B27F-52ADA280A68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1020" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -180,6 +180,27 @@
   </si>
   <si>
     <t>3) NA.</t>
+  </si>
+  <si>
+    <t>I update my database queries</t>
+  </si>
+  <si>
+    <t>Help to backend team for queries</t>
+  </si>
+  <si>
+    <t>Preparing for workshop prsentation process</t>
+  </si>
+  <si>
+    <t>Today I'm present the back4app uses and how it will work</t>
+  </si>
+  <si>
+    <t>Done the prsentation and working on project for next week</t>
+  </si>
+  <si>
+    <t>We are prepare the PPT slides for next  presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pending on the PPT Slides </t>
   </si>
 </sst>
 </file>
@@ -737,7 +758,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1359,9 +1380,15 @@
       <c r="A20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1387,9 +1414,15 @@
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1">
       <c r="A21" s="10"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1415,9 +1448,15 @@
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1">
       <c r="A22" s="11"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>

</xml_diff>